<commit_message>
Info about encryption system added. Compilation into document started
</commit_message>
<xml_diff>
--- a/Comparison.xlsx
+++ b/Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saman\Desktop\Secure Software Engineering\Secure-Software-Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A1E0B85-2A83-495D-81D8-1443DB334CA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9096159-CED2-4A20-B9F8-C3119A60A24F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AB23A71E-E23F-458C-86B2-7F3C412D1F0E}"/>
+    <workbookView xWindow="1995" yWindow="1245" windowWidth="7500" windowHeight="12675" xr2:uid="{AB23A71E-E23F-458C-86B2-7F3C412D1F0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Comparison of Encryption Techniques</t>
   </si>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>Elliptical Curve Techniques</t>
+  </si>
+  <si>
+    <t>5MB: 0.038s</t>
+  </si>
+  <si>
+    <t>It is the new AES</t>
+  </si>
+  <si>
+    <t>5MB: 0.00204s</t>
   </si>
 </sst>
 </file>
@@ -237,20 +246,20 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -574,75 +583,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075AAD73-5D66-4794-9518-89E1E99F9307}">
   <dimension ref="A1:AC47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="K16" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4:U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -679,211 +688,243 @@
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5" t="s">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5" t="s">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5" t="s">
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5" t="s">
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5" t="s">
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="G5" s="5">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="G5" s="2">
         <v>8</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="P5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="S9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
-      <c r="W19" s="6"/>
-      <c r="X19" s="6"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
-      <c r="X20" s="6"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
@@ -891,147 +932,147 @@
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5" t="s">
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5" t="s">
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5" t="s">
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="5"/>
-      <c r="V21" s="5"/>
-      <c r="W21" s="5"/>
-      <c r="X21" s="5"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
-      <c r="P43" s="3"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="6"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="6"/>
+      <c r="P44" s="6"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
@@ -1061,28 +1102,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="A32:C33"/>
-    <mergeCell ref="A19:X20"/>
-    <mergeCell ref="D9:F10"/>
-    <mergeCell ref="D7:F8"/>
-    <mergeCell ref="D17:F18"/>
-    <mergeCell ref="G7:I8"/>
-    <mergeCell ref="A22:C23"/>
-    <mergeCell ref="A24:C25"/>
-    <mergeCell ref="A26:C27"/>
-    <mergeCell ref="A28:C29"/>
-    <mergeCell ref="A30:C31"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="S21:U21"/>
-    <mergeCell ref="V21:X21"/>
-    <mergeCell ref="G5:I6"/>
+  <mergeCells count="41">
     <mergeCell ref="A1:AC2"/>
     <mergeCell ref="A43:P44"/>
     <mergeCell ref="A4:C4"/>
@@ -1099,6 +1119,31 @@
     <mergeCell ref="M4:O4"/>
     <mergeCell ref="P4:R4"/>
     <mergeCell ref="S4:U4"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="S21:U21"/>
+    <mergeCell ref="V21:X21"/>
+    <mergeCell ref="G5:I6"/>
+    <mergeCell ref="J9:L10"/>
+    <mergeCell ref="J7:L8"/>
+    <mergeCell ref="P5:R6"/>
+    <mergeCell ref="S9:U10"/>
+    <mergeCell ref="A32:C33"/>
+    <mergeCell ref="A19:X20"/>
+    <mergeCell ref="D9:F10"/>
+    <mergeCell ref="D7:F8"/>
+    <mergeCell ref="D17:F18"/>
+    <mergeCell ref="G7:I8"/>
+    <mergeCell ref="A22:C23"/>
+    <mergeCell ref="A24:C25"/>
+    <mergeCell ref="A26:C27"/>
+    <mergeCell ref="A28:C29"/>
+    <mergeCell ref="A30:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Documentation of Symmetric encryption into pdf
</commit_message>
<xml_diff>
--- a/Comparison.xlsx
+++ b/Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saman\Desktop\Secure Software Engineering\Secure-Software-Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9096159-CED2-4A20-B9F8-C3119A60A24F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6F194E-2A9B-44F8-95FE-EE5F69A6C133}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1995" yWindow="1245" windowWidth="7500" windowHeight="12675" xr2:uid="{AB23A71E-E23F-458C-86B2-7F3C412D1F0E}"/>
   </bookViews>
@@ -246,22 +246,22 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -583,104 +583,104 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075AAD73-5D66-4794-9518-89E1E99F9307}">
   <dimension ref="A1:AC47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="S4" sqref="S4:U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -688,243 +688,243 @@
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2" t="s">
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2" t="s">
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2" t="s">
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2" t="s">
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="G5" s="2">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="G5" s="6">
         <v>8</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="P5" s="2" t="s">
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="P5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="J9" s="2" t="s">
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="J9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="S9" s="2" t="s">
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="S9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
@@ -932,147 +932,147 @@
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2" t="s">
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2" t="s">
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2" t="s">
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2" t="s">
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
-      <c r="X21" s="2"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
-      <c r="M43" s="6"/>
-      <c r="N43" s="6"/>
-      <c r="O43" s="6"/>
-      <c r="P43" s="6"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
-      <c r="M44" s="6"/>
-      <c r="N44" s="6"/>
-      <c r="O44" s="6"/>
-      <c r="P44" s="6"/>
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
@@ -1103,6 +1103,31 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="A32:C33"/>
+    <mergeCell ref="A19:X20"/>
+    <mergeCell ref="D9:F10"/>
+    <mergeCell ref="D7:F8"/>
+    <mergeCell ref="D17:F18"/>
+    <mergeCell ref="G7:I8"/>
+    <mergeCell ref="A22:C23"/>
+    <mergeCell ref="A24:C25"/>
+    <mergeCell ref="A26:C27"/>
+    <mergeCell ref="A28:C29"/>
+    <mergeCell ref="A30:C31"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="S21:U21"/>
+    <mergeCell ref="V21:X21"/>
+    <mergeCell ref="G5:I6"/>
+    <mergeCell ref="J9:L10"/>
+    <mergeCell ref="J7:L8"/>
+    <mergeCell ref="P5:R6"/>
+    <mergeCell ref="S9:U10"/>
     <mergeCell ref="A1:AC2"/>
     <mergeCell ref="A43:P44"/>
     <mergeCell ref="A4:C4"/>
@@ -1119,31 +1144,6 @@
     <mergeCell ref="M4:O4"/>
     <mergeCell ref="P4:R4"/>
     <mergeCell ref="S4:U4"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="S21:U21"/>
-    <mergeCell ref="V21:X21"/>
-    <mergeCell ref="G5:I6"/>
-    <mergeCell ref="J9:L10"/>
-    <mergeCell ref="J7:L8"/>
-    <mergeCell ref="P5:R6"/>
-    <mergeCell ref="S9:U10"/>
-    <mergeCell ref="A32:C33"/>
-    <mergeCell ref="A19:X20"/>
-    <mergeCell ref="D9:F10"/>
-    <mergeCell ref="D7:F8"/>
-    <mergeCell ref="D17:F18"/>
-    <mergeCell ref="G7:I8"/>
-    <mergeCell ref="A22:C23"/>
-    <mergeCell ref="A24:C25"/>
-    <mergeCell ref="A26:C27"/>
-    <mergeCell ref="A28:C29"/>
-    <mergeCell ref="A30:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>